<commit_message>
added web, android application
</commit_message>
<xml_diff>
--- a/Web/data.xlsx
+++ b/Web/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>Time</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>NODE2</t>
+  </si>
+  <si>
+    <t>2019-04-09 16:22:16</t>
   </si>
 </sst>
 </file>
@@ -389,7 +392,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -445,6 +448,20 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <printOptions gridLines="false" gridLinesSet="true"/>

</xml_diff>